<commit_message>
Updated for fixed/parity bits
</commit_message>
<xml_diff>
--- a/rfid/Keri.xlsx
+++ b/rfid/Keri.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/62f5ee83cc1a8a33/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{22C35EF8-ACEF-4910-B936-CD49FB67836F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A58B5DED-3CF8-416C-92A2-8EAFAF0E7C95}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{59235342-D838-484D-8C21-261DA04BA54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A5503EF-0A0D-419C-9E45-4151F58DF2A6}"/>
   <bookViews>
     <workbookView xWindow="1005" yWindow="3105" windowWidth="28687" windowHeight="11333" xr2:uid="{9F4778D3-973F-44DE-A00C-3281388C6088}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+  <si>
+    <t>KERI</t>
+  </si>
   <si>
     <t>CARD</t>
   </si>
@@ -47,17 +50,41 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>KERI</t>
-  </si>
-  <si>
     <t>RESULT</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>PARITY</t>
+  </si>
+  <si>
+    <t>https://github.com/Next-Flip/Momentum-Firmware/blob/dev/lib/lfrfid/protocols/protocol_keri.c</t>
+  </si>
+  <si>
+    <t>https://github.com/RfidResearchGroup/proxmark3/blob/3ce68d4df918ef738686e7b63181dbe19809edd9/client/src/cmdlfkeri.c</t>
+  </si>
+  <si>
+    <t>MAIN ALGO FROM</t>
+  </si>
+  <si>
+    <t>FIXED/PARITY FROM</t>
+  </si>
+  <si>
+    <t>ENTER YOUR FC AND CARD NUMBER IN CELLS B5 and B6. THE SPREADSHEET WILL CALCULATE THE HEX IN CELL B10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORE INFO - </t>
+  </si>
+  <si>
+    <t>https://github.com/jamisonderek/flipper-zero-tutorials/tree/main/rfid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +96,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,15 +139,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -160,10 +206,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,17 +525,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CE751B-5C8B-4C51-A3BB-245C14A5BD9A}">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" customWidth="1"/>
-    <col min="8" max="28" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="28" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.73046875" bestFit="1" customWidth="1"/>
     <col min="30" max="32" width="2.73046875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="7.73046875" bestFit="1" customWidth="1"/>
@@ -509,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H1" s="1">
         <v>32</v>
@@ -609,287 +654,389 @@
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="R2">
+      <c r="A2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AQ2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="R3">
         <v>10</v>
       </c>
-      <c r="S2">
+      <c r="S3">
         <v>6</v>
       </c>
-      <c r="T2">
+      <c r="T3">
         <v>25</v>
       </c>
-      <c r="U2">
+      <c r="U3">
         <v>23</v>
       </c>
-      <c r="V2">
+      <c r="V3">
         <v>11</v>
       </c>
-      <c r="W2">
+      <c r="W3">
         <v>8</v>
       </c>
-      <c r="X2">
+      <c r="X3">
         <v>17</v>
       </c>
-      <c r="Y2">
+      <c r="Y3">
         <v>27</v>
       </c>
-      <c r="Z2">
+      <c r="Z3">
         <v>4</v>
       </c>
-      <c r="AA2">
+      <c r="AA3">
         <v>5</v>
       </c>
-      <c r="AB2">
+      <c r="AB3">
         <v>19</v>
       </c>
-      <c r="AC2">
+      <c r="AC3">
         <v>16</v>
       </c>
-      <c r="AD2">
+      <c r="AD3">
         <v>29</v>
       </c>
-      <c r="AE2">
+      <c r="AE3">
         <v>12</v>
       </c>
-      <c r="AF2">
+      <c r="AF3">
         <v>15</v>
       </c>
-      <c r="AG2">
+      <c r="AG3">
         <v>9</v>
       </c>
-      <c r="AH2">
+      <c r="AH3">
         <v>7</v>
       </c>
-      <c r="AI2">
+      <c r="AI3">
         <v>20</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ3">
         <v>28</v>
       </c>
-      <c r="AK2">
+      <c r="AK3">
         <v>26</v>
       </c>
-      <c r="AL2">
+      <c r="AL3">
         <v>21</v>
       </c>
-      <c r="AM2">
+      <c r="AM3">
         <v>14</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="AI3">
-        <v>24</v>
-      </c>
-      <c r="AJ3">
-        <v>22</v>
-      </c>
-      <c r="AK3">
-        <v>18</v>
-      </c>
-      <c r="AL3">
-        <v>30</v>
-      </c>
-      <c r="AM3">
-        <v>13</v>
       </c>
       <c r="AQ3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
-        <f>DEC2BIN(MOD($B4,256),8)</f>
-        <v>00000001</v>
-      </c>
       <c r="AI4">
-        <f>IF(MID($F4,9-AI$1,1)="1",2^AI3,0)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AJ4">
-        <f>IF(MID($F4,9-AJ$1,1)="1",2^AJ3,0)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="AK4">
-        <f>IF(MID($F4,9-AK$1,1)="1",2^AK3,0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AL4">
-        <f>IF(MID($F4,9-AL$1,1)="1",2^AL3,0)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AM4">
-        <f>IF(MID($F4,9-AM$1,1)="1",2^AM3,0)</f>
-        <v>8192</v>
-      </c>
-      <c r="AO4">
-        <f>SUM(H4:AM4)</f>
-        <v>8192</v>
-      </c>
-      <c r="AP4" t="str">
-        <f>DEC2HEX(AO4, 8)</f>
-        <v>00002000</v>
+        <v>13</v>
       </c>
       <c r="AQ4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="str">
-        <f>DEC2BIN(MOD($B5/(256*256), 256),8)</f>
-        <v>00000000</v>
-      </c>
-      <c r="E5" t="str">
-        <f>DEC2BIN(MOD($B5/256, 256),8)</f>
-        <v>00000000</v>
+        <v>17</v>
       </c>
       <c r="F5" t="str">
         <f>DEC2BIN(MOD($B5,256),8)</f>
-        <v>00000001</v>
-      </c>
-      <c r="R5">
-        <f t="shared" ref="R5:W5" si="0">IF(MID($D5,25-R$1,1)="1",2^R2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="S5">
+        <v>00010001</v>
+      </c>
+      <c r="AI5">
+        <f>IF(MID($F5,9-AI$1,1)="1",2^AI4,0)</f>
+        <v>16777216</v>
+      </c>
+      <c r="AJ5">
+        <f>IF(MID($F5,9-AJ$1,1)="1",2^AJ4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <f>IF(MID($F5,9-AK$1,1)="1",2^AK4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <f>IF(MID($F5,9-AL$1,1)="1",2^AL4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <f>IF(MID($F5,9-AM$1,1)="1",2^AM4,0)</f>
+        <v>8192</v>
+      </c>
+      <c r="AO5">
+        <f>SUM(H5:AM5)</f>
+        <v>16785408</v>
+      </c>
+      <c r="AP5" t="str">
+        <f>DEC2HEX(AO5, 8)</f>
+        <v>01002000</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1337</v>
+      </c>
+      <c r="D6" t="str">
+        <f>DEC2BIN(MOD($B6/(256*256), 256),8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="E6" t="str">
+        <f>DEC2BIN(MOD($B6/256, 256),8)</f>
+        <v>00000101</v>
+      </c>
+      <c r="F6" t="str">
+        <f>DEC2BIN(MOD($B6,256),8)</f>
+        <v>00111001</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ref="R6:W6" si="0">IF(MID($D6,25-R$1,1)="1",2^R3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="S6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T5">
+      <c r="T6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U5">
+      <c r="U6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V5">
+      <c r="V6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W5">
+      <c r="W6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X5">
-        <f>IF(MID($E5,17-X$1,1)="1",2^X2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <f t="shared" ref="Y5:AE5" si="1">IF(MID($E5,17-Y$1,1)="1",2^Y2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z5">
+      <c r="X6">
+        <f>IF(MID($E6,17-X$1,1)="1",2^X3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ref="Y6:AE6" si="1">IF(MID($E6,17-Y$1,1)="1",2^Y3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA5">
+      <c r="AA6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB5">
+      <c r="AB6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC5">
+      <c r="AC6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AD5">
+        <v>65536</v>
+      </c>
+      <c r="AD6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE5">
+      <c r="AE6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <f>IF(MID($F5,9-AF$1,1)="1",2^AF2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <f t="shared" ref="AG5:AM5" si="2">IF(MID($F5,9-AG$1,1)="1",2^AG2,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AH5">
+        <v>4096</v>
+      </c>
+      <c r="AF6">
+        <f>IF(MID($F6,9-AF$1,1)="1",2^AF3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" ref="AG6:AM6" si="2">IF(MID($F6,9-AG$1,1)="1",2^AG3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AI5">
+        <v>128</v>
+      </c>
+      <c r="AI6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AJ5">
+        <v>1048576</v>
+      </c>
+      <c r="AJ6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AK5">
+        <v>268435456</v>
+      </c>
+      <c r="AK6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AL5">
+      <c r="AL6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AM5">
+      <c r="AM6">
         <f t="shared" si="2"/>
         <v>16384</v>
       </c>
-      <c r="AO5">
-        <f>SUM(H5:AM5)</f>
-        <v>16384</v>
-      </c>
-      <c r="AP5" t="str">
-        <f>DEC2HEX(AO5, 8)</f>
-        <v>00004000</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.45">
       <c r="AO6">
-        <f>AO4+AO5</f>
-        <v>24576</v>
+        <f>SUM(H6:AM6)</f>
+        <v>269570176</v>
       </c>
       <c r="AP6" t="str">
         <f>DEC2HEX(AO6, 8)</f>
-        <v>00006000</v>
+        <v>10115080</v>
       </c>
       <c r="AQ6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="1"/>
+      <c r="M7">
+        <f>2^M2</f>
+        <v>8</v>
+      </c>
+      <c r="N7">
+        <f>2^N2</f>
+        <v>2147483648</v>
+      </c>
+      <c r="AO7">
+        <f>SUM(H7:AM7)</f>
+        <v>2147483656</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <f>MOD(LEN(_xlfn.REGEXREPLACE(_xlfn.REGEXREPLACE(DEC2HEX(SUM(AO5:AO7)), "[236789CD]", "O"),"[^O]","")),2)</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>MOD(LEN(_xlfn.REGEXREPLACE(_xlfn.REGEXREPLACE(DEC2HEX(SUM(AO5:AO7)), "[02578ADF]", "O"),"[^O]",""))+1,2)</f>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f>E8*2^K2</f>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f>D8*2^L2</f>
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <f>SUM(H8:AM8)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="AO9">
+        <f>AO5+AO6+AO7+AO8</f>
+        <v>2433839241</v>
+      </c>
+      <c r="AP9" t="str">
+        <f>DEC2HEX(AO9, 8)</f>
+        <v>91117089</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="str">
-        <f>AP6</f>
-        <v>00006000</v>
+      <c r="B10" s="2" t="str">
+        <f>AP9</f>
+        <v>91117089</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.45">
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B4">
+  <conditionalFormatting sqref="B5">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>31</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5">
+  <conditionalFormatting sqref="B6:B7">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>4194303</formula>
     </cfRule>
@@ -900,7 +1047,12 @@
       <formula>8388607</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D14" r:id="rId1" xr:uid="{C7CD762F-F1BF-4E97-A554-AF5DA62515BF}"/>
+    <hyperlink ref="D13" r:id="rId2" xr:uid="{36E93600-D7AD-471B-BBC7-8A19955F2C47}"/>
+    <hyperlink ref="D17" r:id="rId3" xr:uid="{522FE8A8-6C22-4093-8BBE-7460784851A5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>